<commit_message>
🔧build(stimuli): make dot distinctive
Dots are now more far away for cross now.

Signed-off-by: Liang Zhang <psychelzh@outlook.com>
</commit_message>
<xml_diff>
--- a/config/stimuli.xlsx
+++ b/config/stimuli.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="467">
   <si>
     <t>stim</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -871,6 +871,564 @@
   </si>
   <si>
     <t>0.31-0.20</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>group_note</t>
+  </si>
+  <si>
+    <t>第一象限</t>
+  </si>
+  <si>
+    <t>第二象限</t>
+  </si>
+  <si>
+    <t>第三象限</t>
+  </si>
+  <si>
+    <t>第四象限</t>
+  </si>
+  <si>
+    <t>stim_id</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>stim</t>
+  </si>
+  <si>
+    <t>0.90-0.15</t>
+  </si>
+  <si>
+    <t>0.66-0.38</t>
+  </si>
+  <si>
+    <t>0.77-0.56</t>
+  </si>
+  <si>
+    <t>0.85-0.76</t>
+  </si>
+  <si>
+    <t>0.86-0.50</t>
+  </si>
+  <si>
+    <t>1.00-0.32</t>
+  </si>
+  <si>
+    <t>0.86-0.68</t>
+  </si>
+  <si>
+    <t>0.82-0.45</t>
+  </si>
+  <si>
+    <t>0.82-0.64</t>
+  </si>
+  <si>
+    <t>0.84-0.52</t>
+  </si>
+  <si>
+    <t>0.85-0.27</t>
+  </si>
+  <si>
+    <t>0.82-0.46</t>
+  </si>
+  <si>
+    <t>0.61-0.51</t>
+  </si>
+  <si>
+    <t>0.73-0.66</t>
+  </si>
+  <si>
+    <t>0.99-0.73</t>
+  </si>
+  <si>
+    <t>0.68-0.50</t>
+  </si>
+  <si>
+    <t>0.84-0.59</t>
+  </si>
+  <si>
+    <t>0.96-0.91</t>
+  </si>
+  <si>
+    <t>0.96-0.55</t>
+  </si>
+  <si>
+    <t>0.69-0.68</t>
+  </si>
+  <si>
+    <t>0.79-0.23</t>
+  </si>
+  <si>
+    <t>0.81-0.92</t>
+  </si>
+  <si>
+    <t>0.42-0.91</t>
+  </si>
+  <si>
+    <t>0.57-0.65</t>
+  </si>
+  <si>
+    <t>0.22-0.91</t>
+  </si>
+  <si>
+    <t>0.52-0.97</t>
+  </si>
+  <si>
+    <t>0.63-0.64</t>
+  </si>
+  <si>
+    <t>0.34-0.77</t>
+  </si>
+  <si>
+    <t>0.44-0.59</t>
+  </si>
+  <si>
+    <t>0.76-0.87</t>
+  </si>
+  <si>
+    <t>0.33-0.87</t>
+  </si>
+  <si>
+    <t>0.77-0.92</t>
+  </si>
+  <si>
+    <t>0.59-0.64</t>
+  </si>
+  <si>
+    <t>0.72-0.84</t>
+  </si>
+  <si>
+    <t>0.67-0.93</t>
+  </si>
+  <si>
+    <t>0.21-0.82</t>
+  </si>
+  <si>
+    <t>0.46-0.64</t>
+  </si>
+  <si>
+    <t>0.19-0.94</t>
+  </si>
+  <si>
+    <t>0.77-0.80</t>
+  </si>
+  <si>
+    <t>0.60-0.68</t>
+  </si>
+  <si>
+    <t>0.26-0.81</t>
+  </si>
+  <si>
+    <t>0.16-0.84</t>
+  </si>
+  <si>
+    <t>0.08-0.81</t>
+  </si>
+  <si>
+    <t>0.18-0.61</t>
+  </si>
+  <si>
+    <t>0.09-0.14</t>
+  </si>
+  <si>
+    <t>0.02-0.63</t>
+  </si>
+  <si>
+    <t>0.27-0.67</t>
+  </si>
+  <si>
+    <t>0.33-0.60</t>
+  </si>
+  <si>
+    <t>0.44-0.55</t>
+  </si>
+  <si>
+    <t>0.19-0.71</t>
+  </si>
+  <si>
+    <t>0.15-0.22</t>
+  </si>
+  <si>
+    <t>0.22-0.54</t>
+  </si>
+  <si>
+    <t>0.22-0.48</t>
+  </si>
+  <si>
+    <t>0.05-0.69</t>
+  </si>
+  <si>
+    <t>0.12-0.28</t>
+  </si>
+  <si>
+    <t>0.24-0.72</t>
+  </si>
+  <si>
+    <t>0.29-0.68</t>
+  </si>
+  <si>
+    <t>0.07-0.22</t>
+  </si>
+  <si>
+    <t>0.31-0.35</t>
+  </si>
+  <si>
+    <t>0.26-0.54</t>
+  </si>
+  <si>
+    <t>0.21-0.24</t>
+  </si>
+  <si>
+    <t>0.05-0.69</t>
+  </si>
+  <si>
+    <t>0.08-0.16</t>
+  </si>
+  <si>
+    <t>0.72-0.07</t>
+  </si>
+  <si>
+    <t>0.50-0.28</t>
+  </si>
+  <si>
+    <t>0.10-0.09</t>
+  </si>
+  <si>
+    <t>0.72-0.27</t>
+  </si>
+  <si>
+    <t>0.84-0.04</t>
+  </si>
+  <si>
+    <t>0.20-0.20</t>
+  </si>
+  <si>
+    <t>0.46-0.40</t>
+  </si>
+  <si>
+    <t>0.46-0.20</t>
+  </si>
+  <si>
+    <t>0.47-0.37</t>
+  </si>
+  <si>
+    <t>0.78-0.01</t>
+  </si>
+  <si>
+    <t>0.50-0.37</t>
+  </si>
+  <si>
+    <t>0.65-0.28</t>
+  </si>
+  <si>
+    <t>0.25-0.25</t>
+  </si>
+  <si>
+    <t>0.73-0.09</t>
+  </si>
+  <si>
+    <t>0.40-0.09</t>
+  </si>
+  <si>
+    <t>0.56-0.33</t>
+  </si>
+  <si>
+    <t>0.56-0.18</t>
+  </si>
+  <si>
+    <t>0.65-0.07</t>
+  </si>
+  <si>
+    <t>0.50-0.21</t>
+  </si>
+  <si>
+    <t>0.35-0.15</t>
+  </si>
+  <si>
+    <t>0.23-0.00</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>group_note</t>
+  </si>
+  <si>
+    <t>第一象限</t>
+  </si>
+  <si>
+    <t>第二象限</t>
+  </si>
+  <si>
+    <t>第三象限</t>
+  </si>
+  <si>
+    <t>第四象限</t>
+  </si>
+  <si>
+    <t>stim_id</t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>stim</t>
+  </si>
+  <si>
+    <t>0.77-0.56</t>
+  </si>
+  <si>
+    <t>0.86-0.50</t>
+  </si>
+  <si>
+    <t>1.00-0.32</t>
+  </si>
+  <si>
+    <t>0.86-0.68</t>
+  </si>
+  <si>
+    <t>0.82-0.45</t>
+  </si>
+  <si>
+    <t>0.82-0.64</t>
+  </si>
+  <si>
+    <t>0.84-0.52</t>
+  </si>
+  <si>
+    <t>0.85-0.27</t>
+  </si>
+  <si>
+    <t>0.82-0.46</t>
+  </si>
+  <si>
+    <t>0.99-0.73</t>
+  </si>
+  <si>
+    <t>0.68-0.50</t>
+  </si>
+  <si>
+    <t>0.84-0.59</t>
+  </si>
+  <si>
+    <t>0.96-0.55</t>
+  </si>
+  <si>
+    <t>0.88-0.38</t>
+  </si>
+  <si>
+    <t>0.86-0.54</t>
+  </si>
+  <si>
+    <t>0.71-0.51</t>
+  </si>
+  <si>
+    <t>0.66-0.46</t>
+  </si>
+  <si>
+    <t>0.98-0.40</t>
+  </si>
+  <si>
+    <t>0.75-0.36</t>
+  </si>
+  <si>
+    <t>0.74-0.36</t>
+  </si>
+  <si>
+    <t>0.75-0.41</t>
+  </si>
+  <si>
+    <t>0.46-0.64</t>
+  </si>
+  <si>
+    <t>0.19-0.94</t>
+  </si>
+  <si>
+    <t>0.61-0.99</t>
+  </si>
+  <si>
+    <t>0.71-0.94</t>
+  </si>
+  <si>
+    <t>0.47-0.74</t>
+  </si>
+  <si>
+    <t>0.32-0.81</t>
+  </si>
+  <si>
+    <t>0.37-0.93</t>
+  </si>
+  <si>
+    <t>0.67-0.83</t>
+  </si>
+  <si>
+    <t>0.54-0.85</t>
+  </si>
+  <si>
+    <t>0.52-0.67</t>
+  </si>
+  <si>
+    <t>0.15-0.96</t>
+  </si>
+  <si>
+    <t>0.52-0.89</t>
+  </si>
+  <si>
+    <t>0.60-0.74</t>
+  </si>
+  <si>
+    <t>0.69-0.88</t>
+  </si>
+  <si>
+    <t>0.13-0.99</t>
+  </si>
+  <si>
+    <t>0.27-0.87</t>
+  </si>
+  <si>
+    <t>0.55-0.77</t>
+  </si>
+  <si>
+    <t>0.38-0.91</t>
+  </si>
+  <si>
+    <t>0.51-0.90</t>
+  </si>
+  <si>
+    <t>0.61-0.90</t>
+  </si>
+  <si>
+    <t>0.66-0.89</t>
+  </si>
+  <si>
+    <t>0.25-0.55</t>
+  </si>
+  <si>
+    <t>0.08-0.46</t>
+  </si>
+  <si>
+    <t>0.27-0.58</t>
+  </si>
+  <si>
+    <t>0.16-0.46</t>
+  </si>
+  <si>
+    <t>0.08-0.19</t>
+  </si>
+  <si>
+    <t>0.31-0.55</t>
+  </si>
+  <si>
+    <t>0.30-0.55</t>
+  </si>
+  <si>
+    <t>0.01-0.13</t>
+  </si>
+  <si>
+    <t>0.31-0.48</t>
+  </si>
+  <si>
+    <t>0.19-0.64</t>
+  </si>
+  <si>
+    <t>0.02-0.51</t>
+  </si>
+  <si>
+    <t>0.07-0.60</t>
+  </si>
+  <si>
+    <t>0.04-0.54</t>
+  </si>
+  <si>
+    <t>0.06-0.26</t>
+  </si>
+  <si>
+    <t>0.07-0.45</t>
+  </si>
+  <si>
+    <t>0.12-0.37</t>
+  </si>
+  <si>
+    <t>0.19-0.71</t>
+  </si>
+  <si>
+    <t>0.06-0.32</t>
+  </si>
+  <si>
+    <t>0.06-0.27</t>
+  </si>
+  <si>
+    <t>0.30-0.55</t>
+  </si>
+  <si>
+    <t>0.23-0.51</t>
+  </si>
+  <si>
+    <t>0.44-0.29</t>
+  </si>
+  <si>
+    <t>0.65-0.20</t>
+  </si>
+  <si>
+    <t>0.64-0.13</t>
+  </si>
+  <si>
+    <t>0.54-0.36</t>
+  </si>
+  <si>
+    <t>0.51-0.21</t>
+  </si>
+  <si>
+    <t>0.56-0.10</t>
+  </si>
+  <si>
+    <t>0.41-0.29</t>
+  </si>
+  <si>
+    <t>0.37-0.24</t>
+  </si>
+  <si>
+    <t>0.47-0.12</t>
+  </si>
+  <si>
+    <t>0.33-0.04</t>
+  </si>
+  <si>
+    <t>0.76-0.09</t>
+  </si>
+  <si>
+    <t>0.12-0.00</t>
+  </si>
+  <si>
+    <t>0.63-0.04</t>
+  </si>
+  <si>
+    <t>0.48-0.21</t>
+  </si>
+  <si>
+    <t>0.72-0.13</t>
+  </si>
+  <si>
+    <t>0.45-0.05</t>
+  </si>
+  <si>
+    <t>0.37-0.12</t>
+  </si>
+  <si>
+    <t>0.53-0.08</t>
+  </si>
+  <si>
+    <t>0.17-0.05</t>
+  </si>
+  <si>
+    <t>0.65-0.22</t>
+  </si>
+  <si>
+    <t>0.67-0.09</t>
   </si>
   <si>
     <t>group</t>
@@ -920,7 +1478,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -929,17 +1487,21 @@
       <diagonal/>
     </border>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -4257,19 +4819,19 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="0" t="s">
-        <v>188</v>
+        <v>374</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>189</v>
+        <v>375</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>190</v>
+        <v>376</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>275</v>
+        <v>461</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>276</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
@@ -4280,13 +4842,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>191</v>
+        <v>377</v>
       </c>
       <c r="D2" s="0">
         <v>1</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
@@ -4297,13 +4859,13 @@
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>192</v>
+        <v>378</v>
       </c>
       <c r="D3" s="0">
         <v>1</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.25">
@@ -4314,13 +4876,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>193</v>
+        <v>379</v>
       </c>
       <c r="D4" s="0">
         <v>1</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.25">
@@ -4331,13 +4893,13 @@
         <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>194</v>
+        <v>380</v>
       </c>
       <c r="D5" s="0">
         <v>1</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.25">
@@ -4348,13 +4910,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>195</v>
+        <v>381</v>
       </c>
       <c r="D6" s="0">
         <v>1</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
@@ -4365,13 +4927,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>196</v>
+        <v>382</v>
       </c>
       <c r="D7" s="0">
         <v>1</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
@@ -4382,13 +4944,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>197</v>
+        <v>383</v>
       </c>
       <c r="D8" s="0">
         <v>1</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
@@ -4399,13 +4961,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>198</v>
+        <v>384</v>
       </c>
       <c r="D9" s="0">
         <v>1</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
@@ -4416,13 +4978,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>199</v>
+        <v>385</v>
       </c>
       <c r="D10" s="0">
         <v>1</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
@@ -4433,13 +4995,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>200</v>
+        <v>386</v>
       </c>
       <c r="D11" s="0">
         <v>1</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
@@ -4450,13 +5012,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>201</v>
+        <v>387</v>
       </c>
       <c r="D12" s="0">
         <v>1</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
@@ -4467,13 +5029,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>202</v>
+        <v>388</v>
       </c>
       <c r="D13" s="0">
         <v>1</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
@@ -4484,13 +5046,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>203</v>
+        <v>389</v>
       </c>
       <c r="D14" s="0">
         <v>1</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.25">
@@ -4501,13 +5063,13 @@
         <v>4</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>204</v>
+        <v>390</v>
       </c>
       <c r="D15" s="0">
         <v>1</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
@@ -4518,13 +5080,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>205</v>
+        <v>391</v>
       </c>
       <c r="D16" s="0">
         <v>1</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
@@ -4535,13 +5097,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>206</v>
+        <v>392</v>
       </c>
       <c r="D17" s="0">
         <v>1</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
@@ -4552,13 +5114,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>207</v>
+        <v>393</v>
       </c>
       <c r="D18" s="0">
         <v>1</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
@@ -4569,13 +5131,13 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>208</v>
+        <v>394</v>
       </c>
       <c r="D19" s="0">
         <v>1</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
@@ -4586,13 +5148,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>209</v>
+        <v>395</v>
       </c>
       <c r="D20" s="0">
         <v>1</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
@@ -4603,13 +5165,13 @@
         <v>6</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>210</v>
+        <v>396</v>
       </c>
       <c r="D21" s="0">
         <v>1</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.25">
@@ -4620,13 +5182,13 @@
         <v>6</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>211</v>
+        <v>397</v>
       </c>
       <c r="D22" s="0">
         <v>1</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>277</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.25">
@@ -4637,13 +5199,13 @@
         <v>0</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>212</v>
+        <v>398</v>
       </c>
       <c r="D23" s="0">
         <v>2</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.25">
@@ -4654,13 +5216,13 @@
         <v>0</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>213</v>
+        <v>399</v>
       </c>
       <c r="D24" s="0">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" x14ac:dyDescent="0.25">
@@ -4671,13 +5233,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>214</v>
+        <v>400</v>
       </c>
       <c r="D25" s="0">
         <v>2</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="26" x14ac:dyDescent="0.25">
@@ -4688,13 +5250,13 @@
         <v>1</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>215</v>
+        <v>401</v>
       </c>
       <c r="D26" s="0">
         <v>2</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" x14ac:dyDescent="0.25">
@@ -4705,13 +5267,13 @@
         <v>1</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>216</v>
+        <v>402</v>
       </c>
       <c r="D27" s="0">
         <v>2</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="28" x14ac:dyDescent="0.25">
@@ -4722,13 +5284,13 @@
         <v>1</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>217</v>
+        <v>403</v>
       </c>
       <c r="D28" s="0">
         <v>2</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" x14ac:dyDescent="0.25">
@@ -4739,13 +5301,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>218</v>
+        <v>404</v>
       </c>
       <c r="D29" s="0">
         <v>2</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" x14ac:dyDescent="0.25">
@@ -4756,13 +5318,13 @@
         <v>2</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>219</v>
+        <v>405</v>
       </c>
       <c r="D30" s="0">
         <v>2</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="31" x14ac:dyDescent="0.25">
@@ -4773,13 +5335,13 @@
         <v>2</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>220</v>
+        <v>406</v>
       </c>
       <c r="D31" s="0">
         <v>2</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" x14ac:dyDescent="0.25">
@@ -4790,13 +5352,13 @@
         <v>3</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>221</v>
+        <v>407</v>
       </c>
       <c r="D32" s="0">
         <v>2</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" x14ac:dyDescent="0.25">
@@ -4807,13 +5369,13 @@
         <v>3</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>222</v>
+        <v>408</v>
       </c>
       <c r="D33" s="0">
         <v>2</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="34" x14ac:dyDescent="0.25">
@@ -4824,13 +5386,13 @@
         <v>3</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>223</v>
+        <v>409</v>
       </c>
       <c r="D34" s="0">
         <v>2</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" x14ac:dyDescent="0.25">
@@ -4841,13 +5403,13 @@
         <v>4</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>224</v>
+        <v>410</v>
       </c>
       <c r="D35" s="0">
         <v>2</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" x14ac:dyDescent="0.25">
@@ -4858,13 +5420,13 @@
         <v>4</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>225</v>
+        <v>411</v>
       </c>
       <c r="D36" s="0">
         <v>2</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" x14ac:dyDescent="0.25">
@@ -4875,13 +5437,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>226</v>
+        <v>412</v>
       </c>
       <c r="D37" s="0">
         <v>2</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="38" x14ac:dyDescent="0.25">
@@ -4892,13 +5454,13 @@
         <v>5</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>227</v>
+        <v>413</v>
       </c>
       <c r="D38" s="0">
         <v>2</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" x14ac:dyDescent="0.25">
@@ -4909,13 +5471,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>228</v>
+        <v>414</v>
       </c>
       <c r="D39" s="0">
         <v>2</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" x14ac:dyDescent="0.25">
@@ -4926,13 +5488,13 @@
         <v>5</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>229</v>
+        <v>415</v>
       </c>
       <c r="D40" s="0">
         <v>2</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" x14ac:dyDescent="0.25">
@@ -4943,13 +5505,13 @@
         <v>6</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>230</v>
+        <v>416</v>
       </c>
       <c r="D41" s="0">
         <v>2</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" x14ac:dyDescent="0.25">
@@ -4960,13 +5522,13 @@
         <v>6</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>231</v>
+        <v>417</v>
       </c>
       <c r="D42" s="0">
         <v>2</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="43" x14ac:dyDescent="0.25">
@@ -4977,13 +5539,13 @@
         <v>6</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>232</v>
+        <v>418</v>
       </c>
       <c r="D43" s="0">
         <v>2</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>278</v>
+        <v>464</v>
       </c>
     </row>
     <row r="44" x14ac:dyDescent="0.25">
@@ -4994,13 +5556,13 @@
         <v>0</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>233</v>
+        <v>419</v>
       </c>
       <c r="D44" s="0">
         <v>3</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" x14ac:dyDescent="0.25">
@@ -5011,13 +5573,13 @@
         <v>0</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>234</v>
+        <v>420</v>
       </c>
       <c r="D45" s="0">
         <v>3</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" x14ac:dyDescent="0.25">
@@ -5028,13 +5590,13 @@
         <v>0</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>235</v>
+        <v>421</v>
       </c>
       <c r="D46" s="0">
         <v>3</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="47" x14ac:dyDescent="0.25">
@@ -5045,13 +5607,13 @@
         <v>1</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>236</v>
+        <v>422</v>
       </c>
       <c r="D47" s="0">
         <v>3</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="48" x14ac:dyDescent="0.25">
@@ -5062,13 +5624,13 @@
         <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>237</v>
+        <v>423</v>
       </c>
       <c r="D48" s="0">
         <v>3</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="49" x14ac:dyDescent="0.25">
@@ -5079,13 +5641,13 @@
         <v>1</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>238</v>
+        <v>424</v>
       </c>
       <c r="D49" s="0">
         <v>3</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="50" x14ac:dyDescent="0.25">
@@ -5096,13 +5658,13 @@
         <v>2</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>239</v>
+        <v>425</v>
       </c>
       <c r="D50" s="0">
         <v>3</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" x14ac:dyDescent="0.25">
@@ -5113,13 +5675,13 @@
         <v>2</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>240</v>
+        <v>426</v>
       </c>
       <c r="D51" s="0">
         <v>3</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="52" x14ac:dyDescent="0.25">
@@ -5130,13 +5692,13 @@
         <v>2</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>241</v>
+        <v>427</v>
       </c>
       <c r="D52" s="0">
         <v>3</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="53" x14ac:dyDescent="0.25">
@@ -5147,13 +5709,13 @@
         <v>3</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>242</v>
+        <v>428</v>
       </c>
       <c r="D53" s="0">
         <v>3</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="54" x14ac:dyDescent="0.25">
@@ -5164,13 +5726,13 @@
         <v>3</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>243</v>
+        <v>429</v>
       </c>
       <c r="D54" s="0">
         <v>3</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="55" x14ac:dyDescent="0.25">
@@ -5181,13 +5743,13 @@
         <v>3</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>244</v>
+        <v>430</v>
       </c>
       <c r="D55" s="0">
         <v>3</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="56" x14ac:dyDescent="0.25">
@@ -5198,13 +5760,13 @@
         <v>4</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>245</v>
+        <v>431</v>
       </c>
       <c r="D56" s="0">
         <v>3</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" x14ac:dyDescent="0.25">
@@ -5215,13 +5777,13 @@
         <v>4</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>246</v>
+        <v>432</v>
       </c>
       <c r="D57" s="0">
         <v>3</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" x14ac:dyDescent="0.25">
@@ -5232,13 +5794,13 @@
         <v>4</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>247</v>
+        <v>433</v>
       </c>
       <c r="D58" s="0">
         <v>3</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" x14ac:dyDescent="0.25">
@@ -5249,13 +5811,13 @@
         <v>5</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="D59" s="0">
         <v>3</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" x14ac:dyDescent="0.25">
@@ -5266,13 +5828,13 @@
         <v>5</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>249</v>
+        <v>435</v>
       </c>
       <c r="D60" s="0">
         <v>3</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" x14ac:dyDescent="0.25">
@@ -5283,13 +5845,13 @@
         <v>5</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>250</v>
+        <v>436</v>
       </c>
       <c r="D61" s="0">
         <v>3</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="62" x14ac:dyDescent="0.25">
@@ -5300,13 +5862,13 @@
         <v>6</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>251</v>
+        <v>437</v>
       </c>
       <c r="D62" s="0">
         <v>3</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="63" x14ac:dyDescent="0.25">
@@ -5317,13 +5879,13 @@
         <v>6</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>252</v>
+        <v>438</v>
       </c>
       <c r="D63" s="0">
         <v>3</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="64" x14ac:dyDescent="0.25">
@@ -5334,13 +5896,13 @@
         <v>6</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>253</v>
+        <v>439</v>
       </c>
       <c r="D64" s="0">
         <v>3</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>279</v>
+        <v>465</v>
       </c>
     </row>
     <row r="65" x14ac:dyDescent="0.25">
@@ -5351,13 +5913,13 @@
         <v>0</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>254</v>
+        <v>440</v>
       </c>
       <c r="D65" s="0">
         <v>4</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="66" x14ac:dyDescent="0.25">
@@ -5368,13 +5930,13 @@
         <v>0</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>255</v>
+        <v>441</v>
       </c>
       <c r="D66" s="0">
         <v>4</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="67" x14ac:dyDescent="0.25">
@@ -5385,13 +5947,13 @@
         <v>0</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>256</v>
+        <v>442</v>
       </c>
       <c r="D67" s="0">
         <v>4</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="68" x14ac:dyDescent="0.25">
@@ -5402,13 +5964,13 @@
         <v>1</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>257</v>
+        <v>443</v>
       </c>
       <c r="D68" s="0">
         <v>4</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="69" x14ac:dyDescent="0.25">
@@ -5419,13 +5981,13 @@
         <v>1</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>258</v>
+        <v>444</v>
       </c>
       <c r="D69" s="0">
         <v>4</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="70" x14ac:dyDescent="0.25">
@@ -5436,13 +5998,13 @@
         <v>1</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>259</v>
+        <v>445</v>
       </c>
       <c r="D70" s="0">
         <v>4</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="71" x14ac:dyDescent="0.25">
@@ -5453,13 +6015,13 @@
         <v>2</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>260</v>
+        <v>446</v>
       </c>
       <c r="D71" s="0">
         <v>4</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="72" x14ac:dyDescent="0.25">
@@ -5470,13 +6032,13 @@
         <v>2</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>261</v>
+        <v>447</v>
       </c>
       <c r="D72" s="0">
         <v>4</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="73" x14ac:dyDescent="0.25">
@@ -5487,13 +6049,13 @@
         <v>2</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>262</v>
+        <v>448</v>
       </c>
       <c r="D73" s="0">
         <v>4</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="74" x14ac:dyDescent="0.25">
@@ -5504,13 +6066,13 @@
         <v>3</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>263</v>
+        <v>449</v>
       </c>
       <c r="D74" s="0">
         <v>4</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="75" x14ac:dyDescent="0.25">
@@ -5521,13 +6083,13 @@
         <v>3</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>264</v>
+        <v>450</v>
       </c>
       <c r="D75" s="0">
         <v>4</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="76" x14ac:dyDescent="0.25">
@@ -5538,13 +6100,13 @@
         <v>3</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>265</v>
+        <v>451</v>
       </c>
       <c r="D76" s="0">
         <v>4</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="77" x14ac:dyDescent="0.25">
@@ -5555,13 +6117,13 @@
         <v>4</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>266</v>
+        <v>452</v>
       </c>
       <c r="D77" s="0">
         <v>4</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="78" x14ac:dyDescent="0.25">
@@ -5572,13 +6134,13 @@
         <v>4</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>267</v>
+        <v>453</v>
       </c>
       <c r="D78" s="0">
         <v>4</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="79" x14ac:dyDescent="0.25">
@@ -5589,13 +6151,13 @@
         <v>4</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>268</v>
+        <v>454</v>
       </c>
       <c r="D79" s="0">
         <v>4</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="80" x14ac:dyDescent="0.25">
@@ -5606,13 +6168,13 @@
         <v>5</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>269</v>
+        <v>455</v>
       </c>
       <c r="D80" s="0">
         <v>4</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="81" x14ac:dyDescent="0.25">
@@ -5623,13 +6185,13 @@
         <v>5</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>270</v>
+        <v>456</v>
       </c>
       <c r="D81" s="0">
         <v>4</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="82" x14ac:dyDescent="0.25">
@@ -5640,13 +6202,13 @@
         <v>5</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>271</v>
+        <v>457</v>
       </c>
       <c r="D82" s="0">
         <v>4</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="83" x14ac:dyDescent="0.25">
@@ -5657,13 +6219,13 @@
         <v>6</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>272</v>
+        <v>458</v>
       </c>
       <c r="D83" s="0">
         <v>4</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="84" x14ac:dyDescent="0.25">
@@ -5674,13 +6236,13 @@
         <v>6</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>273</v>
+        <v>459</v>
       </c>
       <c r="D84" s="0">
         <v>4</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
     <row r="85" x14ac:dyDescent="0.25">
@@ -5691,13 +6253,13 @@
         <v>6</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>274</v>
+        <v>460</v>
       </c>
       <c r="D85" s="0">
         <v>4</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>280</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>